<commit_message>
trinomial test in excell
</commit_message>
<xml_diff>
--- a/mturk/trinomial test.xlsx
+++ b/mturk/trinomial test.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isekulic/proj/USi-2.0/mturk/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{579FC1DD-0013-3749-88A2-F92E03E28D11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BEA676C-A4D1-C24F-A286-19F966618945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{6411E0B8-FC2D-FE4D-AA71-246907804B54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId2"/>
+    <externalReference r:id="rId3"/>
   </externalReferences>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -61,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="15">
   <si>
     <t>single turn</t>
   </si>
@@ -88,6 +89,24 @@
   </si>
   <si>
     <t>sum</t>
+  </si>
+  <si>
+    <t>multi turn</t>
+  </si>
+  <si>
+    <t>swap 16 and 18 for p-value</t>
+  </si>
+  <si>
+    <t>Assignment</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>Perc</t>
+  </si>
+  <si>
+    <t>Oleg:</t>
   </si>
 </sst>
 </file>
@@ -216,7 +235,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -504,7 +523,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -512,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11566FDE-338B-C645-9BCD-A07E6BF7DF92}">
-  <dimension ref="B3:H9"/>
+  <dimension ref="B3:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -523,7 +542,7 @@
     <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -532,7 +551,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B4" s="1"/>
       <c r="C4" s="2" t="s">
         <v>1</v>
@@ -550,7 +569,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
@@ -575,7 +594,7 @@
         <v>1.6793644012863051E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
@@ -600,7 +619,7 @@
         <v>3.0917605640410207E-4</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
         <v>1</v>
@@ -613,7 +632,7 @@
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
@@ -638,7 +657,7 @@
         <v>5.5742714736195291E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>5</v>
       </c>
@@ -661,6 +680,292 @@
       <c r="H9" cm="1">
         <f t="array" ref="H9">[1]!TRINOM_TEST(G9/2,E9/2,F9/2,1)</f>
         <v>8.9245867010474041E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B11" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B12" s="1"/>
+      <c r="C12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="1">
+        <v>40</v>
+      </c>
+      <c r="D13" s="1">
+        <v>16</v>
+      </c>
+      <c r="E13" s="1">
+        <v>33</v>
+      </c>
+      <c r="F13" s="1">
+        <f>SUM(C13:E13)</f>
+        <v>89</v>
+      </c>
+      <c r="G13">
+        <f>C13-D13</f>
+        <v>24</v>
+      </c>
+      <c r="H13" cm="1">
+        <f t="array" ref="H13">[1]!TRINOM_TEST(G13/2,E13/2,F13/2,1)</f>
+        <v>1.4562279432960103E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="1">
+        <v>55</v>
+      </c>
+      <c r="D14" s="1">
+        <v>11</v>
+      </c>
+      <c r="E14" s="1">
+        <v>23</v>
+      </c>
+      <c r="F14" s="1">
+        <f>SUM(C14:E14)</f>
+        <v>89</v>
+      </c>
+      <c r="G14">
+        <f t="shared" ref="G14" si="1">C14-D14</f>
+        <v>44</v>
+      </c>
+      <c r="H14" cm="1">
+        <f t="array" ref="H14">[1]!TRINOM_TEST(G14/2,E14/2,F14/2,1)</f>
+        <v>5.2211943263199095E-5</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B15" s="1"/>
+      <c r="C15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="1">
+        <v>16</v>
+      </c>
+      <c r="D16" s="1">
+        <v>18</v>
+      </c>
+      <c r="E16" s="1">
+        <v>31</v>
+      </c>
+      <c r="F16" s="1">
+        <f>SUM(C16:E16)</f>
+        <v>65</v>
+      </c>
+      <c r="G16">
+        <f t="shared" ref="G16:G17" si="2">C16-D16</f>
+        <v>-2</v>
+      </c>
+      <c r="H16" t="e" cm="1">
+        <f t="array" ref="H16">[1]!TRINOM_TEST(G16/2,E16/2,F16/2,1)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="1">
+        <v>17</v>
+      </c>
+      <c r="D17" s="1">
+        <v>10</v>
+      </c>
+      <c r="E17" s="1">
+        <v>38</v>
+      </c>
+      <c r="F17" s="1">
+        <f>SUM(C17:E17)</f>
+        <v>65</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="H17" cm="1">
+        <f t="array" ref="H17">[1]!TRINOM_TEST(G17/2,E17/2,F17/2,1)</f>
+        <v>0.1654129398184857</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C23">
+        <v>60</v>
+      </c>
+      <c r="D23">
+        <v>16</v>
+      </c>
+      <c r="E23">
+        <v>24</v>
+      </c>
+      <c r="F23">
+        <f>SUM(C23:E23)</f>
+        <v>100</v>
+      </c>
+      <c r="G23">
+        <f>C23-D23</f>
+        <v>44</v>
+      </c>
+      <c r="H23" cm="1">
+        <f t="array" ref="H23">[1]!TRINOM_TEST(G23/2,E23/2,F23/2,1)</f>
+        <v>1.9991543251709562E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C24">
+        <v>29</v>
+      </c>
+      <c r="D24">
+        <v>28</v>
+      </c>
+      <c r="E24">
+        <v>43</v>
+      </c>
+      <c r="F24">
+        <f>SUM(C24:E24)</f>
+        <v>100</v>
+      </c>
+      <c r="G24">
+        <f>C24-D24</f>
+        <v>1</v>
+      </c>
+      <c r="H24" cm="1">
+        <f t="array" ref="H24">[1]!TRINOM_TEST(G24/2,E24/2,F24/2,1)</f>
+        <v>0.53758208293285181</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B5F516-2609-4B44-80D5-B4B1A35DA063}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>63</v>
+      </c>
+      <c r="C2">
+        <v>0.15</v>
+      </c>
+      <c r="D2">
+        <f>B2*C2</f>
+        <v>9.4499999999999993</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>99.5</v>
+      </c>
+      <c r="C3">
+        <v>0.2</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D5" si="0">B3*C3</f>
+        <v>19.900000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>78</v>
+      </c>
+      <c r="C4">
+        <v>0.25</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>19.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>24</v>
+      </c>
+      <c r="C5">
+        <v>0.4</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>9.6000000000000014</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <f>SUM(D2:D5)</f>
+        <v>58.45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>